<commit_message>
Adiciona o projeto no GitHUB
</commit_message>
<xml_diff>
--- a/contatos.xlsx
+++ b/contatos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduar\Documents\Códigos\BOT WHATSAPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321C6BF3-AA2A-4074-9DE7-39FD3B5A41E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D815C2E-DEA7-4BC3-8DF6-77E7784D4BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
     <t>Telefone</t>
   </si>
   <si>
-    <t>STEPHANIE</t>
+    <t>PESSOA 1</t>
   </si>
 </sst>
 </file>
@@ -354,7 +354,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -375,7 +375,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>62993759908</v>
+        <v>99999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>